<commit_message>
updated code to implement builder pattern
</commit_message>
<xml_diff>
--- a/excel/XLSXExample.xlsx
+++ b/excel/XLSXExample.xlsx
@@ -188,21 +188,41 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -220,77 +240,77 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" t="s" s="1">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="1">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="2">
+      <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="3">
+      <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="4">
+      <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="5">
+      <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15">
-      <c r="C15" t="s" s="10">
+      <c r="C15" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="12">
+      <c r="A17" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" t="s" s="6">
+      <c r="B19" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" t="n" s="6">
+      <c r="B21" s="6" t="n">
         <v>23.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" t="n" s="7">
+      <c r="B23" s="7" t="n">
         <v>84.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="B25" t="n" s="9">
+      <c r="B25" s="9" t="n">
         <v>1284.25416</v>
       </c>
     </row>
     <row r="27">
-      <c r="B27" t="n" s="8">
+      <c r="B27" s="8" t="n">
         <v>1284.0</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s" s="11">
+      <c r="A29" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s" s="11">
+      <c r="A31" s="11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update merged region style copy
</commit_message>
<xml_diff>
--- a/excel/XLSXExample.xlsx
+++ b/excel/XLSXExample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Primary Header Style</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>Secret Link2</t>
+  </si>
+  <si>
+    <t>merged region1</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>merged region88</t>
   </si>
 </sst>
 </file>
@@ -55,7 +64,7 @@
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -116,6 +125,11 @@
       <color indexed="8"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
       <name val="Tahoma"/>
       <sz val="10.0"/>
       <color indexed="12"/>
@@ -129,7 +143,7 @@
       <b val="true"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,8 +160,22 @@
         <fgColor indexed="54"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="64"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -181,11 +209,189 @@
         <color indexed="8"/>
       </right>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
+        <color indexed="8"/>
+      </right>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
+        <color indexed="8"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
+        <color indexed="8"/>
+      </right>
+      <top style="thick">
+        <color indexed="8"/>
+      </top>
+    </border>
+    <border/>
+    <border>
+      <right style="thick"/>
+    </border>
+    <border>
+      <right style="thick"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thick"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
+        <color indexed="8"/>
+      </right>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
+        <color indexed="8"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thick"/>
+    </border>
+    <border>
+      <top style="thick"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <top style="thick"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thick"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thick">
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thick"/>
+      <top style="thick"/>
+    </border>
+    <border>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
+        <color indexed="8"/>
+      </right>
+      <top style="thick"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
+        <color indexed="8"/>
+      </right>
+      <top style="thick">
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment horizontal="center" vertical="bottom"/>
@@ -217,11 +423,26 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -229,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C31"/>
+  <dimension ref="A3:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -275,7 +496,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -305,18 +526,34 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="12" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="33">
+      <c r="B33" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="16"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A5:C5"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A29" r:id="rId1"/>

</xml_diff>